<commit_message>
added ConRod Drawing for manufacture
</commit_message>
<xml_diff>
--- a/Bill of Materials/ConRods.xlsx
+++ b/Bill of Materials/ConRods.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xbria\MotionBase\Bill of Materials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mac\Desktop\MotionBase\Bill of Materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="105" yWindow="60" windowWidth="6735" windowHeight="8880"/>
+    <workbookView xWindow="108" yWindow="60" windowWidth="6732" windowHeight="8880"/>
   </bookViews>
   <sheets>
     <sheet name="Expansion Tube Team" sheetId="1" r:id="rId1"/>
@@ -892,69 +892,290 @@
     <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -964,234 +1185,13 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0" hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0" hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1538,293 +1538,293 @@
   </sheetPr>
   <dimension ref="A1:J62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="13.15" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1328125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="11.265625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="7.59765625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11.21875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="7.5546875" style="2" customWidth="1"/>
     <col min="4" max="4" width="14" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.73046875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="20.59765625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15.77734375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="20.5546875" style="2" customWidth="1"/>
     <col min="7" max="7" width="40" style="2" customWidth="1"/>
-    <col min="8" max="8" width="17.3984375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="12.59765625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="9.1328125" style="2" hidden="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.1328125" style="2"/>
+    <col min="8" max="8" width="17.44140625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="12.5546875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="9.109375" style="2" hidden="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="74" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="92" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
-      <c r="I1" s="76"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="77"/>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="79"/>
+      <c r="B1" s="93"/>
+      <c r="C1" s="93"/>
+      <c r="D1" s="93"/>
+      <c r="E1" s="93"/>
+      <c r="F1" s="93"/>
+      <c r="G1" s="93"/>
+      <c r="H1" s="93"/>
+      <c r="I1" s="94"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="95"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="97"/>
       <c r="J2" s="11"/>
     </row>
-    <row r="3" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="80"/>
-      <c r="B3" s="81"/>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="82"/>
-    </row>
-    <row r="4" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="91"/>
-      <c r="B4" s="91"/>
-      <c r="C4" s="91"/>
-      <c r="D4" s="91"/>
-      <c r="E4" s="91"/>
-      <c r="F4" s="91"/>
-      <c r="G4" s="91"/>
-      <c r="H4" s="91"/>
-      <c r="I4" s="91"/>
-    </row>
-    <row r="5" spans="1:10" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="102" t="s">
+    <row r="3" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="98"/>
+      <c r="B3" s="99"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="100"/>
+    </row>
+    <row r="4" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="109"/>
+      <c r="B4" s="109"/>
+      <c r="C4" s="109"/>
+      <c r="D4" s="109"/>
+      <c r="E4" s="109"/>
+      <c r="F4" s="109"/>
+      <c r="G4" s="109"/>
+      <c r="H4" s="109"/>
+      <c r="I4" s="109"/>
+    </row>
+    <row r="5" spans="1:10" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="118" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="103"/>
-      <c r="C5" s="104" t="s">
+      <c r="B5" s="119"/>
+      <c r="C5" s="120" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="104"/>
-      <c r="E5" s="104"/>
-      <c r="F5" s="104"/>
-      <c r="G5" s="104"/>
-      <c r="H5" s="104"/>
-      <c r="I5" s="105"/>
-    </row>
-    <row r="6" spans="1:10" ht="11.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="109"/>
-      <c r="B6" s="109"/>
-      <c r="C6" s="109"/>
-      <c r="D6" s="109"/>
-      <c r="E6" s="109"/>
-      <c r="F6" s="109"/>
-      <c r="G6" s="109"/>
-      <c r="H6" s="109"/>
-      <c r="I6" s="109"/>
-    </row>
-    <row r="7" spans="1:10" ht="24.75" x14ac:dyDescent="0.35">
-      <c r="A7" s="92" t="s">
+      <c r="D5" s="120"/>
+      <c r="E5" s="120"/>
+      <c r="F5" s="120"/>
+      <c r="G5" s="120"/>
+      <c r="H5" s="120"/>
+      <c r="I5" s="121"/>
+    </row>
+    <row r="6" spans="1:10" ht="11.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="125"/>
+      <c r="B6" s="125"/>
+      <c r="C6" s="125"/>
+      <c r="D6" s="125"/>
+      <c r="E6" s="125"/>
+      <c r="F6" s="125"/>
+      <c r="G6" s="125"/>
+      <c r="H6" s="125"/>
+      <c r="I6" s="125"/>
+    </row>
+    <row r="7" spans="1:10" ht="24.6" x14ac:dyDescent="0.25">
+      <c r="A7" s="110" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="93"/>
-      <c r="C7" s="93"/>
-      <c r="D7" s="93"/>
-      <c r="E7" s="93"/>
-      <c r="F7" s="93"/>
-      <c r="G7" s="93"/>
-      <c r="H7" s="93"/>
-      <c r="I7" s="94"/>
-    </row>
-    <row r="8" spans="1:10" s="17" customFormat="1" ht="11.45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="77"/>
-      <c r="B8" s="78"/>
-      <c r="C8" s="78"/>
-      <c r="D8" s="78"/>
-      <c r="E8" s="78"/>
-      <c r="F8" s="78"/>
-      <c r="G8" s="78"/>
-      <c r="H8" s="78"/>
-      <c r="I8" s="79"/>
-    </row>
-    <row r="9" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="100" t="s">
+      <c r="B7" s="111"/>
+      <c r="C7" s="111"/>
+      <c r="D7" s="111"/>
+      <c r="E7" s="111"/>
+      <c r="F7" s="111"/>
+      <c r="G7" s="111"/>
+      <c r="H7" s="111"/>
+      <c r="I7" s="112"/>
+    </row>
+    <row r="8" spans="1:10" s="17" customFormat="1" ht="11.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="95"/>
+      <c r="B8" s="96"/>
+      <c r="C8" s="96"/>
+      <c r="D8" s="96"/>
+      <c r="E8" s="96"/>
+      <c r="F8" s="96"/>
+      <c r="G8" s="96"/>
+      <c r="H8" s="96"/>
+      <c r="I8" s="97"/>
+    </row>
+    <row r="9" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="101"/>
-      <c r="C9" s="132" t="s">
+      <c r="B9" s="62"/>
+      <c r="C9" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="133"/>
-      <c r="E9" s="133"/>
-      <c r="F9" s="133"/>
-      <c r="G9" s="134"/>
-      <c r="H9" s="141"/>
-      <c r="I9" s="142"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="64"/>
+      <c r="F9" s="64"/>
+      <c r="G9" s="65"/>
+      <c r="H9" s="69"/>
+      <c r="I9" s="70"/>
       <c r="J9" s="4"/>
     </row>
-    <row r="10" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="106"/>
-      <c r="B10" s="107"/>
-      <c r="C10" s="107"/>
-      <c r="D10" s="107"/>
-      <c r="E10" s="107"/>
-      <c r="F10" s="107"/>
-      <c r="G10" s="107"/>
-      <c r="H10" s="107"/>
-      <c r="I10" s="108"/>
-    </row>
-    <row r="11" spans="1:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="100" t="s">
+    <row r="10" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="122"/>
+      <c r="B10" s="123"/>
+      <c r="C10" s="123"/>
+      <c r="D10" s="123"/>
+      <c r="E10" s="123"/>
+      <c r="F10" s="123"/>
+      <c r="G10" s="123"/>
+      <c r="H10" s="123"/>
+      <c r="I10" s="124"/>
+    </row>
+    <row r="11" spans="1:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="101"/>
-      <c r="C11" s="129" t="s">
+      <c r="B11" s="62"/>
+      <c r="C11" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="130"/>
-      <c r="E11" s="130"/>
-      <c r="F11" s="130"/>
-      <c r="G11" s="131"/>
-      <c r="H11" s="143"/>
-      <c r="I11" s="144"/>
-    </row>
-    <row r="12" spans="1:10" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="138"/>
-      <c r="B12" s="139"/>
-      <c r="C12" s="139"/>
-      <c r="D12" s="139"/>
-      <c r="E12" s="139"/>
-      <c r="F12" s="139"/>
-      <c r="G12" s="139"/>
-      <c r="H12" s="139"/>
-      <c r="I12" s="140"/>
-    </row>
-    <row r="13" spans="1:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="100" t="s">
+      <c r="D11" s="59"/>
+      <c r="E11" s="59"/>
+      <c r="F11" s="59"/>
+      <c r="G11" s="60"/>
+      <c r="H11" s="71"/>
+      <c r="I11" s="72"/>
+    </row>
+    <row r="12" spans="1:10" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="53"/>
+      <c r="B12" s="54"/>
+      <c r="C12" s="54"/>
+      <c r="D12" s="54"/>
+      <c r="E12" s="54"/>
+      <c r="F12" s="54"/>
+      <c r="G12" s="54"/>
+      <c r="H12" s="54"/>
+      <c r="I12" s="55"/>
+    </row>
+    <row r="13" spans="1:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="101"/>
-      <c r="C13" s="135" t="s">
+      <c r="B13" s="62"/>
+      <c r="C13" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="136"/>
-      <c r="E13" s="136"/>
-      <c r="F13" s="136"/>
-      <c r="G13" s="137"/>
-      <c r="H13" s="143"/>
-      <c r="I13" s="144"/>
-    </row>
-    <row r="14" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="138"/>
-      <c r="B14" s="139"/>
-      <c r="C14" s="139"/>
-      <c r="D14" s="139"/>
-      <c r="E14" s="139"/>
-      <c r="F14" s="139"/>
-      <c r="G14" s="139"/>
-      <c r="H14" s="139"/>
-      <c r="I14" s="140"/>
-    </row>
-    <row r="15" spans="1:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="148" t="s">
+      <c r="D13" s="67"/>
+      <c r="E13" s="67"/>
+      <c r="F13" s="67"/>
+      <c r="G13" s="68"/>
+      <c r="H13" s="71"/>
+      <c r="I13" s="72"/>
+    </row>
+    <row r="14" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="53"/>
+      <c r="B14" s="54"/>
+      <c r="C14" s="54"/>
+      <c r="D14" s="54"/>
+      <c r="E14" s="54"/>
+      <c r="F14" s="54"/>
+      <c r="G14" s="54"/>
+      <c r="H14" s="54"/>
+      <c r="I14" s="55"/>
+    </row>
+    <row r="15" spans="1:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="149"/>
-      <c r="C15" s="129"/>
-      <c r="D15" s="130"/>
-      <c r="E15" s="130"/>
-      <c r="F15" s="130"/>
-      <c r="G15" s="131"/>
+      <c r="B15" s="57"/>
+      <c r="C15" s="58"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="59"/>
+      <c r="F15" s="59"/>
+      <c r="G15" s="60"/>
       <c r="H15" s="44"/>
       <c r="I15" s="45"/>
     </row>
-    <row r="16" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="86"/>
-      <c r="B16" s="87"/>
-      <c r="C16" s="87"/>
-      <c r="D16" s="87"/>
-      <c r="E16" s="87"/>
-      <c r="F16" s="87"/>
-      <c r="G16" s="87"/>
-      <c r="H16" s="87"/>
-      <c r="I16" s="88"/>
+    <row r="16" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="104"/>
+      <c r="B16" s="105"/>
+      <c r="C16" s="105"/>
+      <c r="D16" s="105"/>
+      <c r="E16" s="105"/>
+      <c r="F16" s="105"/>
+      <c r="G16" s="105"/>
+      <c r="H16" s="105"/>
+      <c r="I16" s="106"/>
       <c r="J16" s="11"/>
     </row>
-    <row r="17" spans="1:9" s="11" customFormat="1" ht="13.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="89"/>
-      <c r="B17" s="90"/>
-      <c r="C17" s="90"/>
-      <c r="D17" s="90"/>
-      <c r="E17" s="90"/>
-      <c r="F17" s="90"/>
-      <c r="G17" s="90"/>
-      <c r="H17" s="90"/>
-      <c r="I17" s="90"/>
-    </row>
-    <row r="18" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="92" t="s">
+    <row r="17" spans="1:9" s="11" customFormat="1" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="107"/>
+      <c r="B17" s="108"/>
+      <c r="C17" s="108"/>
+      <c r="D17" s="108"/>
+      <c r="E17" s="108"/>
+      <c r="F17" s="108"/>
+      <c r="G17" s="108"/>
+      <c r="H17" s="108"/>
+      <c r="I17" s="108"/>
+    </row>
+    <row r="18" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="110" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="93"/>
-      <c r="C18" s="93"/>
-      <c r="D18" s="93"/>
-      <c r="E18" s="93"/>
-      <c r="F18" s="93"/>
-      <c r="G18" s="93"/>
-      <c r="H18" s="93"/>
-      <c r="I18" s="94"/>
-    </row>
-    <row r="19" spans="1:9" s="17" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="95"/>
-      <c r="B19" s="96"/>
-      <c r="C19" s="96"/>
-      <c r="D19" s="96"/>
-      <c r="E19" s="96"/>
-      <c r="F19" s="96"/>
-      <c r="G19" s="96"/>
-      <c r="H19" s="96"/>
-      <c r="I19" s="97"/>
-    </row>
-    <row r="20" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="111"/>
+      <c r="C18" s="111"/>
+      <c r="D18" s="111"/>
+      <c r="E18" s="111"/>
+      <c r="F18" s="111"/>
+      <c r="G18" s="111"/>
+      <c r="H18" s="111"/>
+      <c r="I18" s="112"/>
+    </row>
+    <row r="19" spans="1:9" s="17" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="113"/>
+      <c r="B19" s="114"/>
+      <c r="C19" s="114"/>
+      <c r="D19" s="114"/>
+      <c r="E19" s="114"/>
+      <c r="F19" s="114"/>
+      <c r="G19" s="114"/>
+      <c r="H19" s="114"/>
+      <c r="I19" s="115"/>
+    </row>
+    <row r="20" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="145">
+      <c r="B20" s="50">
         <f ca="1">TODAY()</f>
-        <v>42466</v>
-      </c>
-      <c r="C20" s="146"/>
-      <c r="D20" s="146"/>
-      <c r="E20" s="147"/>
+        <v>42467</v>
+      </c>
+      <c r="C20" s="51"/>
+      <c r="D20" s="51"/>
+      <c r="E20" s="52"/>
       <c r="F20" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="G20" s="98" t="s">
+      <c r="G20" s="116" t="s">
         <v>32</v>
       </c>
-      <c r="H20" s="99"/>
+      <c r="H20" s="117"/>
       <c r="I20" s="36"/>
     </row>
-    <row r="21" spans="1:9" ht="9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="83"/>
-      <c r="B21" s="84"/>
-      <c r="C21" s="84"/>
-      <c r="D21" s="84"/>
-      <c r="E21" s="84"/>
-      <c r="F21" s="84"/>
-      <c r="G21" s="84"/>
-      <c r="H21" s="84"/>
-      <c r="I21" s="85"/>
-    </row>
-    <row r="22" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="101"/>
+      <c r="B21" s="102"/>
+      <c r="C21" s="102"/>
+      <c r="D21" s="102"/>
+      <c r="E21" s="102"/>
+      <c r="F21" s="102"/>
+      <c r="G21" s="102"/>
+      <c r="H21" s="102"/>
+      <c r="I21" s="103"/>
+    </row>
+    <row r="22" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="37"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -1835,22 +1835,22 @@
       <c r="H22" s="5"/>
       <c r="I22" s="38"/>
     </row>
-    <row r="23" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="110" t="s">
+    <row r="23" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="111"/>
-      <c r="C23" s="118" t="s">
+      <c r="B23" s="74"/>
+      <c r="C23" s="81" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="119"/>
-      <c r="E23" s="119"/>
-      <c r="F23" s="119"/>
-      <c r="G23" s="119"/>
-      <c r="H23" s="120"/>
+      <c r="D23" s="82"/>
+      <c r="E23" s="82"/>
+      <c r="F23" s="82"/>
+      <c r="G23" s="82"/>
+      <c r="H23" s="83"/>
       <c r="I23" s="38"/>
     </row>
-    <row r="24" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="35"/>
       <c r="B24" s="3"/>
       <c r="C24" s="5"/>
@@ -1861,20 +1861,20 @@
       <c r="H24" s="5"/>
       <c r="I24" s="38"/>
     </row>
-    <row r="25" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="110" t="s">
+    <row r="25" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="111"/>
-      <c r="C25" s="121"/>
-      <c r="D25" s="122"/>
-      <c r="E25" s="122"/>
-      <c r="F25" s="122"/>
-      <c r="G25" s="122"/>
-      <c r="H25" s="123"/>
+      <c r="B25" s="74"/>
+      <c r="C25" s="84"/>
+      <c r="D25" s="85"/>
+      <c r="E25" s="85"/>
+      <c r="F25" s="85"/>
+      <c r="G25" s="85"/>
+      <c r="H25" s="86"/>
       <c r="I25" s="38"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="39"/>
       <c r="B26" s="6"/>
       <c r="C26" s="7"/>
@@ -1885,13 +1885,13 @@
       <c r="H26" s="8"/>
       <c r="I26" s="38"/>
     </row>
-    <row r="27" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="112" t="s">
+    <row r="27" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="B27" s="113"/>
-      <c r="C27" s="124"/>
-      <c r="D27" s="125"/>
+      <c r="B27" s="76"/>
+      <c r="C27" s="87"/>
+      <c r="D27" s="88"/>
       <c r="E27" s="41" t="s">
         <v>12</v>
       </c>
@@ -1902,7 +1902,7 @@
       <c r="H27" s="1"/>
       <c r="I27" s="36"/>
     </row>
-    <row r="28" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="39"/>
       <c r="B28" s="6"/>
       <c r="C28" s="9"/>
@@ -1913,20 +1913,20 @@
       <c r="H28" s="8"/>
       <c r="I28" s="38"/>
     </row>
-    <row r="29" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="110" t="s">
+    <row r="29" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="111"/>
-      <c r="C29" s="115"/>
-      <c r="D29" s="116"/>
-      <c r="E29" s="116"/>
-      <c r="F29" s="116"/>
-      <c r="G29" s="116"/>
-      <c r="H29" s="117"/>
+      <c r="B29" s="74"/>
+      <c r="C29" s="78"/>
+      <c r="D29" s="79"/>
+      <c r="E29" s="79"/>
+      <c r="F29" s="79"/>
+      <c r="G29" s="79"/>
+      <c r="H29" s="80"/>
       <c r="I29" s="38"/>
     </row>
-    <row r="30" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="35"/>
       <c r="B30" s="3"/>
       <c r="C30" s="10"/>
@@ -1937,42 +1937,42 @@
       <c r="H30" s="10"/>
       <c r="I30" s="38"/>
     </row>
-    <row r="31" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="110" t="s">
+    <row r="31" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="B31" s="111"/>
-      <c r="C31" s="115"/>
-      <c r="D31" s="116"/>
-      <c r="E31" s="116"/>
-      <c r="F31" s="116"/>
-      <c r="G31" s="116"/>
-      <c r="H31" s="117"/>
+      <c r="B31" s="74"/>
+      <c r="C31" s="78"/>
+      <c r="D31" s="79"/>
+      <c r="E31" s="79"/>
+      <c r="F31" s="79"/>
+      <c r="G31" s="79"/>
+      <c r="H31" s="80"/>
       <c r="I31" s="40"/>
     </row>
-    <row r="32" spans="1:9" ht="13.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="126"/>
-      <c r="B32" s="127"/>
-      <c r="C32" s="127"/>
-      <c r="D32" s="127"/>
-      <c r="E32" s="127"/>
-      <c r="F32" s="127"/>
-      <c r="G32" s="127"/>
-      <c r="H32" s="127"/>
-      <c r="I32" s="128"/>
-    </row>
-    <row r="33" spans="1:9" s="11" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="59"/>
-      <c r="B33" s="59"/>
-      <c r="C33" s="59"/>
-      <c r="D33" s="59"/>
-      <c r="E33" s="59"/>
-      <c r="F33" s="59"/>
-      <c r="G33" s="59"/>
-      <c r="H33" s="59"/>
-      <c r="I33" s="59"/>
-    </row>
-    <row r="34" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" ht="13.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="89"/>
+      <c r="B32" s="90"/>
+      <c r="C32" s="90"/>
+      <c r="D32" s="90"/>
+      <c r="E32" s="90"/>
+      <c r="F32" s="90"/>
+      <c r="G32" s="90"/>
+      <c r="H32" s="90"/>
+      <c r="I32" s="91"/>
+    </row>
+    <row r="33" spans="1:9" s="11" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="129"/>
+      <c r="B33" s="129"/>
+      <c r="C33" s="129"/>
+      <c r="D33" s="129"/>
+      <c r="E33" s="129"/>
+      <c r="F33" s="129"/>
+      <c r="G33" s="129"/>
+      <c r="H33" s="129"/>
+      <c r="I33" s="129"/>
+    </row>
+    <row r="34" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="21" t="s">
         <v>3</v>
       </c>
@@ -1985,11 +1985,11 @@
       <c r="D34" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E34" s="114" t="s">
+      <c r="E34" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="F34" s="114"/>
-      <c r="G34" s="114"/>
+      <c r="F34" s="77"/>
+      <c r="G34" s="77"/>
       <c r="H34" s="21" t="s">
         <v>8</v>
       </c>
@@ -1997,7 +1997,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="45.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="22">
         <v>1</v>
       </c>
@@ -2010,11 +2010,11 @@
       <c r="D35" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="E35" s="64" t="s">
+      <c r="E35" s="134" t="s">
         <v>39</v>
       </c>
-      <c r="F35" s="65"/>
-      <c r="G35" s="65"/>
+      <c r="F35" s="135"/>
+      <c r="G35" s="135"/>
       <c r="H35" s="48">
         <v>9.94</v>
       </c>
@@ -2023,7 +2023,7 @@
         <v>59.64</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="22">
         <v>2</v>
       </c>
@@ -2036,11 +2036,11 @@
       <c r="D36" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="E36" s="64" t="s">
+      <c r="E36" s="134" t="s">
         <v>38</v>
       </c>
-      <c r="F36" s="65"/>
-      <c r="G36" s="65"/>
+      <c r="F36" s="135"/>
+      <c r="G36" s="135"/>
       <c r="H36" s="14">
         <v>9.94</v>
       </c>
@@ -2049,7 +2049,7 @@
         <v>59.64</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="22">
         <v>3</v>
       </c>
@@ -2062,11 +2062,11 @@
       <c r="D37" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="E37" s="64" t="s">
+      <c r="E37" s="134" t="s">
         <v>37</v>
       </c>
-      <c r="F37" s="65"/>
-      <c r="G37" s="65"/>
+      <c r="F37" s="135"/>
+      <c r="G37" s="135"/>
       <c r="H37" s="14">
         <v>6.12</v>
       </c>
@@ -2075,7 +2075,7 @@
         <v>36.72</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="22">
         <v>4</v>
       </c>
@@ -2088,11 +2088,11 @@
       <c r="D38" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="E38" s="64" t="s">
+      <c r="E38" s="134" t="s">
         <v>40</v>
       </c>
-      <c r="F38" s="65"/>
-      <c r="G38" s="65"/>
+      <c r="F38" s="135"/>
+      <c r="G38" s="135"/>
       <c r="H38" s="14">
         <v>6.12</v>
       </c>
@@ -2101,7 +2101,7 @@
         <v>36.72</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="22">
         <v>5</v>
       </c>
@@ -2114,11 +2114,11 @@
       <c r="D39" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="E39" s="50" t="s">
+      <c r="E39" s="143" t="s">
         <v>43</v>
       </c>
-      <c r="F39" s="51"/>
-      <c r="G39" s="52"/>
+      <c r="F39" s="137"/>
+      <c r="G39" s="138"/>
       <c r="H39" s="14">
         <v>78.13</v>
       </c>
@@ -2127,22 +2127,22 @@
         <v>156.26</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="22">
         <v>6</v>
       </c>
       <c r="B40" s="12"/>
       <c r="C40" s="12"/>
       <c r="D40" s="47"/>
-      <c r="E40" s="66"/>
-      <c r="F40" s="51"/>
-      <c r="G40" s="52"/>
+      <c r="E40" s="136"/>
+      <c r="F40" s="137"/>
+      <c r="G40" s="138"/>
       <c r="H40" s="14"/>
       <c r="I40" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="22">
         <v>7</v>
       </c>
@@ -2158,7 +2158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="22">
         <v>8</v>
       </c>
@@ -2174,7 +2174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="22">
         <v>9</v>
       </c>
@@ -2190,7 +2190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="22">
         <v>10</v>
       </c>
@@ -2206,183 +2206,183 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="22">
         <v>11</v>
       </c>
       <c r="B45" s="12"/>
       <c r="C45" s="12"/>
       <c r="D45" s="13"/>
-      <c r="E45" s="50"/>
-      <c r="F45" s="51"/>
-      <c r="G45" s="52"/>
+      <c r="E45" s="143"/>
+      <c r="F45" s="137"/>
+      <c r="G45" s="138"/>
       <c r="H45" s="14"/>
       <c r="I45" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="22">
         <v>12</v>
       </c>
       <c r="B46" s="12"/>
       <c r="C46" s="12"/>
       <c r="D46" s="13"/>
-      <c r="E46" s="50"/>
-      <c r="F46" s="51"/>
-      <c r="G46" s="52"/>
+      <c r="E46" s="143"/>
+      <c r="F46" s="137"/>
+      <c r="G46" s="138"/>
       <c r="H46" s="14"/>
       <c r="I46" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="22">
         <v>13</v>
       </c>
       <c r="B47" s="12"/>
       <c r="C47" s="12"/>
       <c r="D47" s="13"/>
-      <c r="E47" s="50"/>
-      <c r="F47" s="51"/>
-      <c r="G47" s="52"/>
+      <c r="E47" s="143"/>
+      <c r="F47" s="137"/>
+      <c r="G47" s="138"/>
       <c r="H47" s="14"/>
       <c r="I47" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="22">
         <v>14</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="12"/>
       <c r="D48" s="13"/>
-      <c r="E48" s="50"/>
-      <c r="F48" s="51"/>
-      <c r="G48" s="52"/>
+      <c r="E48" s="143"/>
+      <c r="F48" s="137"/>
+      <c r="G48" s="138"/>
       <c r="H48" s="14"/>
       <c r="I48" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="22">
         <v>15</v>
       </c>
       <c r="B49" s="12"/>
       <c r="C49" s="12"/>
       <c r="D49" s="13"/>
-      <c r="E49" s="50"/>
-      <c r="F49" s="51"/>
-      <c r="G49" s="52"/>
+      <c r="E49" s="143"/>
+      <c r="F49" s="137"/>
+      <c r="G49" s="138"/>
       <c r="H49" s="14"/>
       <c r="I49" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="22">
         <v>16</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="12"/>
       <c r="D50" s="13"/>
-      <c r="E50" s="50"/>
-      <c r="F50" s="51"/>
-      <c r="G50" s="52"/>
+      <c r="E50" s="143"/>
+      <c r="F50" s="137"/>
+      <c r="G50" s="138"/>
       <c r="H50" s="14"/>
       <c r="I50" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="22">
         <v>17</v>
       </c>
       <c r="B51" s="12"/>
       <c r="C51" s="12"/>
       <c r="D51" s="13"/>
-      <c r="E51" s="50"/>
-      <c r="F51" s="51"/>
-      <c r="G51" s="52"/>
+      <c r="E51" s="143"/>
+      <c r="F51" s="137"/>
+      <c r="G51" s="138"/>
       <c r="H51" s="14"/>
       <c r="I51" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="22">
         <v>18</v>
       </c>
       <c r="B52" s="12"/>
       <c r="C52" s="12"/>
       <c r="D52" s="13"/>
-      <c r="E52" s="50"/>
-      <c r="F52" s="51"/>
-      <c r="G52" s="52"/>
+      <c r="E52" s="143"/>
+      <c r="F52" s="137"/>
+      <c r="G52" s="138"/>
       <c r="H52" s="14"/>
       <c r="I52" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="22">
         <v>19</v>
       </c>
       <c r="B53" s="12"/>
       <c r="C53" s="12"/>
       <c r="D53" s="13"/>
-      <c r="E53" s="50"/>
-      <c r="F53" s="51"/>
-      <c r="G53" s="52"/>
+      <c r="E53" s="143"/>
+      <c r="F53" s="137"/>
+      <c r="G53" s="138"/>
       <c r="H53" s="14"/>
       <c r="I53" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="22">
         <v>20</v>
       </c>
       <c r="B54" s="15"/>
       <c r="C54" s="15"/>
       <c r="D54" s="15"/>
-      <c r="E54" s="71"/>
-      <c r="F54" s="72"/>
-      <c r="G54" s="73"/>
+      <c r="E54" s="144"/>
+      <c r="F54" s="145"/>
+      <c r="G54" s="146"/>
       <c r="H54" s="16"/>
       <c r="I54" s="23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="53" t="s">
+    <row r="55" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="147" t="s">
         <v>10</v>
       </c>
-      <c r="B55" s="54"/>
-      <c r="C55" s="54"/>
-      <c r="D55" s="54"/>
-      <c r="E55" s="54"/>
-      <c r="F55" s="54"/>
-      <c r="G55" s="54"/>
-      <c r="H55" s="55"/>
+      <c r="B55" s="148"/>
+      <c r="C55" s="148"/>
+      <c r="D55" s="148"/>
+      <c r="E55" s="148"/>
+      <c r="F55" s="148"/>
+      <c r="G55" s="148"/>
+      <c r="H55" s="149"/>
       <c r="I55" s="24">
         <f>SUM(I35:I54)</f>
         <v>348.98</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="25"/>
       <c r="B56" s="26"/>
       <c r="C56" s="26"/>
@@ -2393,44 +2393,44 @@
       <c r="H56" s="26"/>
       <c r="I56" s="27"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A57" s="67" t="s">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="139" t="s">
         <v>11</v>
       </c>
-      <c r="B57" s="68"/>
-      <c r="C57" s="68"/>
-      <c r="D57" s="68"/>
-      <c r="E57" s="69"/>
-      <c r="F57" s="69"/>
-      <c r="G57" s="69"/>
-      <c r="H57" s="69"/>
+      <c r="B57" s="140"/>
+      <c r="C57" s="140"/>
+      <c r="D57" s="140"/>
+      <c r="E57" s="141"/>
+      <c r="F57" s="141"/>
+      <c r="G57" s="141"/>
+      <c r="H57" s="141"/>
       <c r="I57" s="28"/>
     </row>
-    <row r="58" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A58" s="67"/>
-      <c r="B58" s="68"/>
-      <c r="C58" s="68"/>
-      <c r="D58" s="68"/>
-      <c r="E58" s="70"/>
-      <c r="F58" s="70"/>
-      <c r="G58" s="70"/>
-      <c r="H58" s="70"/>
+    <row r="58" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="139"/>
+      <c r="B58" s="140"/>
+      <c r="C58" s="140"/>
+      <c r="D58" s="140"/>
+      <c r="E58" s="142"/>
+      <c r="F58" s="142"/>
+      <c r="G58" s="142"/>
+      <c r="H58" s="142"/>
       <c r="I58" s="28"/>
     </row>
-    <row r="59" spans="1:9" ht="25.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="29"/>
       <c r="B59" s="30"/>
       <c r="C59" s="30"/>
       <c r="D59" s="30"/>
-      <c r="E59" s="60" t="s">
+      <c r="E59" s="130" t="s">
         <v>44</v>
       </c>
-      <c r="F59" s="60"/>
-      <c r="G59" s="60"/>
-      <c r="H59" s="60"/>
+      <c r="F59" s="130"/>
+      <c r="G59" s="130"/>
+      <c r="H59" s="130"/>
       <c r="I59" s="31"/>
     </row>
-    <row r="60" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="11"/>
       <c r="B60" s="11"/>
       <c r="C60" s="11"/>
@@ -2441,57 +2441,56 @@
       <c r="H60" s="11"/>
       <c r="I60" s="11"/>
     </row>
-    <row r="61" spans="1:9" s="11" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="56" t="s">
+    <row r="61" spans="1:9" s="11" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="126" t="s">
         <v>19</v>
       </c>
-      <c r="B61" s="57"/>
-      <c r="C61" s="57"/>
-      <c r="D61" s="58"/>
+      <c r="B61" s="127"/>
+      <c r="C61" s="127"/>
+      <c r="D61" s="128"/>
       <c r="E61" s="32"/>
       <c r="F61" s="32"/>
       <c r="G61" s="32"/>
       <c r="H61" s="32"/>
       <c r="I61" s="33"/>
     </row>
-    <row r="62" spans="1:9" ht="150" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A62" s="61"/>
-      <c r="B62" s="62"/>
-      <c r="C62" s="62"/>
-      <c r="D62" s="62"/>
-      <c r="E62" s="62"/>
-      <c r="F62" s="62"/>
-      <c r="G62" s="62"/>
-      <c r="H62" s="62"/>
-      <c r="I62" s="63"/>
+    <row r="62" spans="1:9" ht="150" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="131"/>
+      <c r="B62" s="132"/>
+      <c r="C62" s="132"/>
+      <c r="D62" s="132"/>
+      <c r="E62" s="132"/>
+      <c r="F62" s="132"/>
+      <c r="G62" s="132"/>
+      <c r="H62" s="132"/>
+      <c r="I62" s="133"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0"/>
   <mergeCells count="63">
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="A14:I14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="A12:I12"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C31:H31"/>
-    <mergeCell ref="C23:H23"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="C25:H25"/>
-    <mergeCell ref="C29:H29"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="A32:I32"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="A55:H55"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="A61:D61"/>
+    <mergeCell ref="A33:I33"/>
+    <mergeCell ref="E59:H59"/>
+    <mergeCell ref="A62:I62"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="A57:D58"/>
+    <mergeCell ref="E57:H58"/>
+    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="E52:G52"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="E54:G54"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="E45:G45"/>
     <mergeCell ref="A1:I3"/>
     <mergeCell ref="A21:I21"/>
     <mergeCell ref="A16:I16"/>
@@ -2508,29 +2507,30 @@
     <mergeCell ref="A6:I6"/>
     <mergeCell ref="A7:I7"/>
     <mergeCell ref="A8:I8"/>
-    <mergeCell ref="A61:D61"/>
-    <mergeCell ref="A33:I33"/>
-    <mergeCell ref="E59:H59"/>
-    <mergeCell ref="A62:I62"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="A57:D58"/>
-    <mergeCell ref="E57:H58"/>
-    <mergeCell ref="E53:G53"/>
-    <mergeCell ref="E52:G52"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="E54:G54"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="A55:H55"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:H31"/>
+    <mergeCell ref="C23:H23"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C25:H25"/>
+    <mergeCell ref="C29:H29"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="A32:I32"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="A12:I12"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="A14:I14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="A13:B13"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <dataValidations count="1">

</xml_diff>

<commit_message>
Updated Drawings. Added PDFs. Added Top and Bottom Triangle BOM
</commit_message>
<xml_diff>
--- a/Bill of Materials/ConRods.xlsx
+++ b/Bill of Materials/ConRods.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mac\Desktop\MotionBase\Bill of Materials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonesdm\Desktop\MotionBase\Bill of Materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="108" yWindow="60" windowWidth="6732" windowHeight="8880"/>
+    <workbookView xWindow="105" yWindow="60" windowWidth="6735" windowHeight="8880"/>
   </bookViews>
   <sheets>
     <sheet name="Expansion Tube Team" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -99,9 +99,6 @@
     <t xml:space="preserve">Phone: </t>
   </si>
   <si>
-    <t xml:space="preserve">   Expansion Tube Project</t>
-  </si>
-  <si>
     <t>Account to Charge:</t>
   </si>
   <si>
@@ -158,12 +155,15 @@
   </si>
   <si>
     <t>Alexander Brown</t>
+  </si>
+  <si>
+    <t>ME395</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
@@ -892,37 +892,154 @@
     <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -931,36 +1048,28 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0" hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0" hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1020,178 +1129,69 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1288,23 +1288,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1340,23 +1323,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1538,293 +1504,293 @@
   </sheetPr>
   <dimension ref="A1:J62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="11.21875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="7.5546875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" style="2" customWidth="1"/>
     <col min="4" max="4" width="14" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.77734375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="20.5546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="20.5703125" style="2" customWidth="1"/>
     <col min="7" max="7" width="40" style="2" customWidth="1"/>
-    <col min="8" max="8" width="17.44140625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="12.5546875" style="2" customWidth="1"/>
-    <col min="10" max="10" width="9.109375" style="2" hidden="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="2"/>
+    <col min="8" max="8" width="17.42578125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="2" hidden="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="92" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="93"/>
-      <c r="C1" s="93"/>
-      <c r="D1" s="93"/>
-      <c r="E1" s="93"/>
-      <c r="F1" s="93"/>
-      <c r="G1" s="93"/>
-      <c r="H1" s="93"/>
-      <c r="I1" s="94"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="95"/>
-      <c r="B2" s="96"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="97"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="76"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="77"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="79"/>
       <c r="J2" s="11"/>
     </row>
-    <row r="3" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="98"/>
-      <c r="B3" s="99"/>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="99"/>
-      <c r="G3" s="99"/>
-      <c r="H3" s="99"/>
-      <c r="I3" s="100"/>
-    </row>
-    <row r="4" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="109"/>
-      <c r="B4" s="109"/>
-      <c r="C4" s="109"/>
-      <c r="D4" s="109"/>
-      <c r="E4" s="109"/>
-      <c r="F4" s="109"/>
-      <c r="G4" s="109"/>
-      <c r="H4" s="109"/>
-      <c r="I4" s="109"/>
-    </row>
-    <row r="5" spans="1:10" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="118" t="s">
+    <row r="3" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="80"/>
+      <c r="B3" s="81"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="81"/>
+      <c r="H3" s="81"/>
+      <c r="I3" s="82"/>
+    </row>
+    <row r="4" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="91"/>
+      <c r="B4" s="91"/>
+      <c r="C4" s="91"/>
+      <c r="D4" s="91"/>
+      <c r="E4" s="91"/>
+      <c r="F4" s="91"/>
+      <c r="G4" s="91"/>
+      <c r="H4" s="91"/>
+      <c r="I4" s="91"/>
+    </row>
+    <row r="5" spans="1:10" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="102" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="119"/>
-      <c r="C5" s="120" t="s">
+      <c r="B5" s="103"/>
+      <c r="C5" s="104" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="104"/>
+      <c r="E5" s="104"/>
+      <c r="F5" s="104"/>
+      <c r="G5" s="104"/>
+      <c r="H5" s="104"/>
+      <c r="I5" s="105"/>
+    </row>
+    <row r="6" spans="1:10" ht="11.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="109"/>
+      <c r="B6" s="109"/>
+      <c r="C6" s="109"/>
+      <c r="D6" s="109"/>
+      <c r="E6" s="109"/>
+      <c r="F6" s="109"/>
+      <c r="G6" s="109"/>
+      <c r="H6" s="109"/>
+      <c r="I6" s="109"/>
+    </row>
+    <row r="7" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A7" s="92" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="93"/>
+      <c r="C7" s="93"/>
+      <c r="D7" s="93"/>
+      <c r="E7" s="93"/>
+      <c r="F7" s="93"/>
+      <c r="G7" s="93"/>
+      <c r="H7" s="93"/>
+      <c r="I7" s="94"/>
+    </row>
+    <row r="8" spans="1:10" s="17" customFormat="1" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="77"/>
+      <c r="B8" s="78"/>
+      <c r="C8" s="78"/>
+      <c r="D8" s="78"/>
+      <c r="E8" s="78"/>
+      <c r="F8" s="78"/>
+      <c r="G8" s="78"/>
+      <c r="H8" s="78"/>
+      <c r="I8" s="79"/>
+    </row>
+    <row r="9" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="100" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="101"/>
+      <c r="C9" s="132" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="133"/>
+      <c r="E9" s="133"/>
+      <c r="F9" s="133"/>
+      <c r="G9" s="134"/>
+      <c r="H9" s="141"/>
+      <c r="I9" s="142"/>
+      <c r="J9" s="4"/>
+    </row>
+    <row r="10" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="106"/>
+      <c r="B10" s="107"/>
+      <c r="C10" s="107"/>
+      <c r="D10" s="107"/>
+      <c r="E10" s="107"/>
+      <c r="F10" s="107"/>
+      <c r="G10" s="107"/>
+      <c r="H10" s="107"/>
+      <c r="I10" s="108"/>
+    </row>
+    <row r="11" spans="1:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="100" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="101"/>
+      <c r="C11" s="129" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="130"/>
+      <c r="E11" s="130"/>
+      <c r="F11" s="130"/>
+      <c r="G11" s="131"/>
+      <c r="H11" s="143"/>
+      <c r="I11" s="144"/>
+    </row>
+    <row r="12" spans="1:10" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="138"/>
+      <c r="B12" s="139"/>
+      <c r="C12" s="139"/>
+      <c r="D12" s="139"/>
+      <c r="E12" s="139"/>
+      <c r="F12" s="139"/>
+      <c r="G12" s="139"/>
+      <c r="H12" s="139"/>
+      <c r="I12" s="140"/>
+    </row>
+    <row r="13" spans="1:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="100" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="101"/>
+      <c r="C13" s="135" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="136"/>
+      <c r="E13" s="136"/>
+      <c r="F13" s="136"/>
+      <c r="G13" s="137"/>
+      <c r="H13" s="143"/>
+      <c r="I13" s="144"/>
+    </row>
+    <row r="14" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="138"/>
+      <c r="B14" s="139"/>
+      <c r="C14" s="139"/>
+      <c r="D14" s="139"/>
+      <c r="E14" s="139"/>
+      <c r="F14" s="139"/>
+      <c r="G14" s="139"/>
+      <c r="H14" s="139"/>
+      <c r="I14" s="140"/>
+    </row>
+    <row r="15" spans="1:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="148" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="120"/>
-      <c r="E5" s="120"/>
-      <c r="F5" s="120"/>
-      <c r="G5" s="120"/>
-      <c r="H5" s="120"/>
-      <c r="I5" s="121"/>
-    </row>
-    <row r="6" spans="1:10" ht="11.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="125"/>
-      <c r="B6" s="125"/>
-      <c r="C6" s="125"/>
-      <c r="D6" s="125"/>
-      <c r="E6" s="125"/>
-      <c r="F6" s="125"/>
-      <c r="G6" s="125"/>
-      <c r="H6" s="125"/>
-      <c r="I6" s="125"/>
-    </row>
-    <row r="7" spans="1:10" ht="24.6" x14ac:dyDescent="0.25">
-      <c r="A7" s="110" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="111"/>
-      <c r="C7" s="111"/>
-      <c r="D7" s="111"/>
-      <c r="E7" s="111"/>
-      <c r="F7" s="111"/>
-      <c r="G7" s="111"/>
-      <c r="H7" s="111"/>
-      <c r="I7" s="112"/>
-    </row>
-    <row r="8" spans="1:10" s="17" customFormat="1" ht="11.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="95"/>
-      <c r="B8" s="96"/>
-      <c r="C8" s="96"/>
-      <c r="D8" s="96"/>
-      <c r="E8" s="96"/>
-      <c r="F8" s="96"/>
-      <c r="G8" s="96"/>
-      <c r="H8" s="96"/>
-      <c r="I8" s="97"/>
-    </row>
-    <row r="9" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="61" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="62"/>
-      <c r="C9" s="63" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="64"/>
-      <c r="E9" s="64"/>
-      <c r="F9" s="64"/>
-      <c r="G9" s="65"/>
-      <c r="H9" s="69"/>
-      <c r="I9" s="70"/>
-      <c r="J9" s="4"/>
-    </row>
-    <row r="10" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="122"/>
-      <c r="B10" s="123"/>
-      <c r="C10" s="123"/>
-      <c r="D10" s="123"/>
-      <c r="E10" s="123"/>
-      <c r="F10" s="123"/>
-      <c r="G10" s="123"/>
-      <c r="H10" s="123"/>
-      <c r="I10" s="124"/>
-    </row>
-    <row r="11" spans="1:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="61" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="62"/>
-      <c r="C11" s="58" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="59"/>
-      <c r="E11" s="59"/>
-      <c r="F11" s="59"/>
-      <c r="G11" s="60"/>
-      <c r="H11" s="71"/>
-      <c r="I11" s="72"/>
-    </row>
-    <row r="12" spans="1:10" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="53"/>
-      <c r="B12" s="54"/>
-      <c r="C12" s="54"/>
-      <c r="D12" s="54"/>
-      <c r="E12" s="54"/>
-      <c r="F12" s="54"/>
-      <c r="G12" s="54"/>
-      <c r="H12" s="54"/>
-      <c r="I12" s="55"/>
-    </row>
-    <row r="13" spans="1:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="61" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="62"/>
-      <c r="C13" s="66" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="67"/>
-      <c r="E13" s="67"/>
-      <c r="F13" s="67"/>
-      <c r="G13" s="68"/>
-      <c r="H13" s="71"/>
-      <c r="I13" s="72"/>
-    </row>
-    <row r="14" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="53"/>
-      <c r="B14" s="54"/>
-      <c r="C14" s="54"/>
-      <c r="D14" s="54"/>
-      <c r="E14" s="54"/>
-      <c r="F14" s="54"/>
-      <c r="G14" s="54"/>
-      <c r="H14" s="54"/>
-      <c r="I14" s="55"/>
-    </row>
-    <row r="15" spans="1:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="56" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="57"/>
-      <c r="C15" s="58"/>
-      <c r="D15" s="59"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="60"/>
+      <c r="B15" s="149"/>
+      <c r="C15" s="129"/>
+      <c r="D15" s="130"/>
+      <c r="E15" s="130"/>
+      <c r="F15" s="130"/>
+      <c r="G15" s="131"/>
       <c r="H15" s="44"/>
       <c r="I15" s="45"/>
     </row>
-    <row r="16" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="104"/>
-      <c r="B16" s="105"/>
-      <c r="C16" s="105"/>
-      <c r="D16" s="105"/>
-      <c r="E16" s="105"/>
-      <c r="F16" s="105"/>
-      <c r="G16" s="105"/>
-      <c r="H16" s="105"/>
-      <c r="I16" s="106"/>
+    <row r="16" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="86"/>
+      <c r="B16" s="87"/>
+      <c r="C16" s="87"/>
+      <c r="D16" s="87"/>
+      <c r="E16" s="87"/>
+      <c r="F16" s="87"/>
+      <c r="G16" s="87"/>
+      <c r="H16" s="87"/>
+      <c r="I16" s="88"/>
       <c r="J16" s="11"/>
     </row>
-    <row r="17" spans="1:9" s="11" customFormat="1" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="107"/>
-      <c r="B17" s="108"/>
-      <c r="C17" s="108"/>
-      <c r="D17" s="108"/>
-      <c r="E17" s="108"/>
-      <c r="F17" s="108"/>
-      <c r="G17" s="108"/>
-      <c r="H17" s="108"/>
-      <c r="I17" s="108"/>
-    </row>
-    <row r="18" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="110" t="s">
+    <row r="17" spans="1:9" s="11" customFormat="1" ht="13.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="89"/>
+      <c r="B17" s="90"/>
+      <c r="C17" s="90"/>
+      <c r="D17" s="90"/>
+      <c r="E17" s="90"/>
+      <c r="F17" s="90"/>
+      <c r="G17" s="90"/>
+      <c r="H17" s="90"/>
+      <c r="I17" s="90"/>
+    </row>
+    <row r="18" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="92" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="111"/>
-      <c r="C18" s="111"/>
-      <c r="D18" s="111"/>
-      <c r="E18" s="111"/>
-      <c r="F18" s="111"/>
-      <c r="G18" s="111"/>
-      <c r="H18" s="111"/>
-      <c r="I18" s="112"/>
-    </row>
-    <row r="19" spans="1:9" s="17" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="113"/>
-      <c r="B19" s="114"/>
-      <c r="C19" s="114"/>
-      <c r="D19" s="114"/>
-      <c r="E19" s="114"/>
-      <c r="F19" s="114"/>
-      <c r="G19" s="114"/>
-      <c r="H19" s="114"/>
-      <c r="I19" s="115"/>
-    </row>
-    <row r="20" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="93"/>
+      <c r="C18" s="93"/>
+      <c r="D18" s="93"/>
+      <c r="E18" s="93"/>
+      <c r="F18" s="93"/>
+      <c r="G18" s="93"/>
+      <c r="H18" s="93"/>
+      <c r="I18" s="94"/>
+    </row>
+    <row r="19" spans="1:9" s="17" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="95"/>
+      <c r="B19" s="96"/>
+      <c r="C19" s="96"/>
+      <c r="D19" s="96"/>
+      <c r="E19" s="96"/>
+      <c r="F19" s="96"/>
+      <c r="G19" s="96"/>
+      <c r="H19" s="96"/>
+      <c r="I19" s="97"/>
+    </row>
+    <row r="20" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="50">
+      <c r="B20" s="145">
         <f ca="1">TODAY()</f>
-        <v>42467</v>
-      </c>
-      <c r="C20" s="51"/>
-      <c r="D20" s="51"/>
-      <c r="E20" s="52"/>
+        <v>42470</v>
+      </c>
+      <c r="C20" s="146"/>
+      <c r="D20" s="146"/>
+      <c r="E20" s="147"/>
       <c r="F20" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="G20" s="116" t="s">
-        <v>32</v>
-      </c>
-      <c r="H20" s="117"/>
+      <c r="G20" s="98" t="s">
+        <v>31</v>
+      </c>
+      <c r="H20" s="99"/>
       <c r="I20" s="36"/>
     </row>
-    <row r="21" spans="1:9" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="101"/>
-      <c r="B21" s="102"/>
-      <c r="C21" s="102"/>
-      <c r="D21" s="102"/>
-      <c r="E21" s="102"/>
-      <c r="F21" s="102"/>
-      <c r="G21" s="102"/>
-      <c r="H21" s="102"/>
-      <c r="I21" s="103"/>
-    </row>
-    <row r="22" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="83"/>
+      <c r="B21" s="84"/>
+      <c r="C21" s="84"/>
+      <c r="D21" s="84"/>
+      <c r="E21" s="84"/>
+      <c r="F21" s="84"/>
+      <c r="G21" s="84"/>
+      <c r="H21" s="84"/>
+      <c r="I21" s="85"/>
+    </row>
+    <row r="22" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="37"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -1835,22 +1801,22 @@
       <c r="H22" s="5"/>
       <c r="I22" s="38"/>
     </row>
-    <row r="23" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="73" t="s">
+    <row r="23" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="110" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="74"/>
-      <c r="C23" s="81" t="s">
-        <v>28</v>
-      </c>
-      <c r="D23" s="82"/>
-      <c r="E23" s="82"/>
-      <c r="F23" s="82"/>
-      <c r="G23" s="82"/>
-      <c r="H23" s="83"/>
+      <c r="B23" s="111"/>
+      <c r="C23" s="118" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="119"/>
+      <c r="E23" s="119"/>
+      <c r="F23" s="119"/>
+      <c r="G23" s="119"/>
+      <c r="H23" s="120"/>
       <c r="I23" s="38"/>
     </row>
-    <row r="24" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="35"/>
       <c r="B24" s="3"/>
       <c r="C24" s="5"/>
@@ -1861,20 +1827,20 @@
       <c r="H24" s="5"/>
       <c r="I24" s="38"/>
     </row>
-    <row r="25" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="73" t="s">
+    <row r="25" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="110" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="74"/>
-      <c r="C25" s="84"/>
-      <c r="D25" s="85"/>
-      <c r="E25" s="85"/>
-      <c r="F25" s="85"/>
-      <c r="G25" s="85"/>
-      <c r="H25" s="86"/>
+      <c r="B25" s="111"/>
+      <c r="C25" s="121"/>
+      <c r="D25" s="122"/>
+      <c r="E25" s="122"/>
+      <c r="F25" s="122"/>
+      <c r="G25" s="122"/>
+      <c r="H25" s="123"/>
       <c r="I25" s="38"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="39"/>
       <c r="B26" s="6"/>
       <c r="C26" s="7"/>
@@ -1885,13 +1851,13 @@
       <c r="H26" s="8"/>
       <c r="I26" s="38"/>
     </row>
-    <row r="27" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="75" t="s">
+    <row r="27" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="112" t="s">
         <v>15</v>
       </c>
-      <c r="B27" s="76"/>
-      <c r="C27" s="87"/>
-      <c r="D27" s="88"/>
+      <c r="B27" s="113"/>
+      <c r="C27" s="124"/>
+      <c r="D27" s="125"/>
       <c r="E27" s="41" t="s">
         <v>12</v>
       </c>
@@ -1902,7 +1868,7 @@
       <c r="H27" s="1"/>
       <c r="I27" s="36"/>
     </row>
-    <row r="28" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="39"/>
       <c r="B28" s="6"/>
       <c r="C28" s="9"/>
@@ -1913,20 +1879,20 @@
       <c r="H28" s="8"/>
       <c r="I28" s="38"/>
     </row>
-    <row r="29" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="73" t="s">
+    <row r="29" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="110" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="74"/>
-      <c r="C29" s="78"/>
-      <c r="D29" s="79"/>
-      <c r="E29" s="79"/>
-      <c r="F29" s="79"/>
-      <c r="G29" s="79"/>
-      <c r="H29" s="80"/>
+      <c r="B29" s="111"/>
+      <c r="C29" s="115"/>
+      <c r="D29" s="116"/>
+      <c r="E29" s="116"/>
+      <c r="F29" s="116"/>
+      <c r="G29" s="116"/>
+      <c r="H29" s="117"/>
       <c r="I29" s="38"/>
     </row>
-    <row r="30" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="35"/>
       <c r="B30" s="3"/>
       <c r="C30" s="10"/>
@@ -1937,42 +1903,42 @@
       <c r="H30" s="10"/>
       <c r="I30" s="38"/>
     </row>
-    <row r="31" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="73" t="s">
+    <row r="31" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="110" t="s">
         <v>14</v>
       </c>
-      <c r="B31" s="74"/>
-      <c r="C31" s="78"/>
-      <c r="D31" s="79"/>
-      <c r="E31" s="79"/>
-      <c r="F31" s="79"/>
-      <c r="G31" s="79"/>
-      <c r="H31" s="80"/>
+      <c r="B31" s="111"/>
+      <c r="C31" s="115"/>
+      <c r="D31" s="116"/>
+      <c r="E31" s="116"/>
+      <c r="F31" s="116"/>
+      <c r="G31" s="116"/>
+      <c r="H31" s="117"/>
       <c r="I31" s="40"/>
     </row>
-    <row r="32" spans="1:9" ht="13.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="89"/>
-      <c r="B32" s="90"/>
-      <c r="C32" s="90"/>
-      <c r="D32" s="90"/>
-      <c r="E32" s="90"/>
-      <c r="F32" s="90"/>
-      <c r="G32" s="90"/>
-      <c r="H32" s="90"/>
-      <c r="I32" s="91"/>
-    </row>
-    <row r="33" spans="1:9" s="11" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="129"/>
-      <c r="B33" s="129"/>
-      <c r="C33" s="129"/>
-      <c r="D33" s="129"/>
-      <c r="E33" s="129"/>
-      <c r="F33" s="129"/>
-      <c r="G33" s="129"/>
-      <c r="H33" s="129"/>
-      <c r="I33" s="129"/>
-    </row>
-    <row r="34" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="13.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="126"/>
+      <c r="B32" s="127"/>
+      <c r="C32" s="127"/>
+      <c r="D32" s="127"/>
+      <c r="E32" s="127"/>
+      <c r="F32" s="127"/>
+      <c r="G32" s="127"/>
+      <c r="H32" s="127"/>
+      <c r="I32" s="128"/>
+    </row>
+    <row r="33" spans="1:9" s="11" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="59"/>
+      <c r="B33" s="59"/>
+      <c r="C33" s="59"/>
+      <c r="D33" s="59"/>
+      <c r="E33" s="59"/>
+      <c r="F33" s="59"/>
+      <c r="G33" s="59"/>
+      <c r="H33" s="59"/>
+      <c r="I33" s="59"/>
+    </row>
+    <row r="34" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="21" t="s">
         <v>3</v>
       </c>
@@ -1985,11 +1951,11 @@
       <c r="D34" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E34" s="77" t="s">
+      <c r="E34" s="114" t="s">
         <v>7</v>
       </c>
-      <c r="F34" s="77"/>
-      <c r="G34" s="77"/>
+      <c r="F34" s="114"/>
+      <c r="G34" s="114"/>
       <c r="H34" s="21" t="s">
         <v>8</v>
       </c>
@@ -1997,7 +1963,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="22">
         <v>1</v>
       </c>
@@ -2005,16 +1971,16 @@
         <v>6</v>
       </c>
       <c r="C35" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D35" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="D35" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="E35" s="134" t="s">
-        <v>39</v>
-      </c>
-      <c r="F35" s="135"/>
-      <c r="G35" s="135"/>
+      <c r="E35" s="64" t="s">
+        <v>38</v>
+      </c>
+      <c r="F35" s="65"/>
+      <c r="G35" s="65"/>
       <c r="H35" s="48">
         <v>9.94</v>
       </c>
@@ -2023,7 +1989,7 @@
         <v>59.64</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="22">
         <v>2</v>
       </c>
@@ -2031,16 +1997,16 @@
         <v>6</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D36" s="47" t="s">
-        <v>35</v>
-      </c>
-      <c r="E36" s="134" t="s">
-        <v>38</v>
-      </c>
-      <c r="F36" s="135"/>
-      <c r="G36" s="135"/>
+        <v>34</v>
+      </c>
+      <c r="E36" s="64" t="s">
+        <v>37</v>
+      </c>
+      <c r="F36" s="65"/>
+      <c r="G36" s="65"/>
       <c r="H36" s="14">
         <v>9.94</v>
       </c>
@@ -2049,7 +2015,7 @@
         <v>59.64</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="22">
         <v>3</v>
       </c>
@@ -2057,16 +2023,16 @@
         <v>6</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D37" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="E37" s="64" t="s">
         <v>36</v>
       </c>
-      <c r="E37" s="134" t="s">
-        <v>37</v>
-      </c>
-      <c r="F37" s="135"/>
-      <c r="G37" s="135"/>
+      <c r="F37" s="65"/>
+      <c r="G37" s="65"/>
       <c r="H37" s="14">
         <v>6.12</v>
       </c>
@@ -2075,7 +2041,7 @@
         <v>36.72</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="22">
         <v>4</v>
       </c>
@@ -2083,16 +2049,16 @@
         <v>6</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D38" s="49" t="s">
-        <v>41</v>
-      </c>
-      <c r="E38" s="134" t="s">
         <v>40</v>
       </c>
-      <c r="F38" s="135"/>
-      <c r="G38" s="135"/>
+      <c r="E38" s="64" t="s">
+        <v>39</v>
+      </c>
+      <c r="F38" s="65"/>
+      <c r="G38" s="65"/>
       <c r="H38" s="14">
         <v>6.12</v>
       </c>
@@ -2101,7 +2067,7 @@
         <v>36.72</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="22">
         <v>5</v>
       </c>
@@ -2109,16 +2075,16 @@
         <v>2</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D39" s="47" t="s">
+        <v>41</v>
+      </c>
+      <c r="E39" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="E39" s="143" t="s">
-        <v>43</v>
-      </c>
-      <c r="F39" s="137"/>
-      <c r="G39" s="138"/>
+      <c r="F39" s="51"/>
+      <c r="G39" s="52"/>
       <c r="H39" s="14">
         <v>78.13</v>
       </c>
@@ -2127,22 +2093,22 @@
         <v>156.26</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="22">
         <v>6</v>
       </c>
       <c r="B40" s="12"/>
       <c r="C40" s="12"/>
       <c r="D40" s="47"/>
-      <c r="E40" s="136"/>
-      <c r="F40" s="137"/>
-      <c r="G40" s="138"/>
+      <c r="E40" s="66"/>
+      <c r="F40" s="51"/>
+      <c r="G40" s="52"/>
       <c r="H40" s="14"/>
       <c r="I40" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="22">
         <v>7</v>
       </c>
@@ -2158,7 +2124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="22">
         <v>8</v>
       </c>
@@ -2174,7 +2140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="22">
         <v>9</v>
       </c>
@@ -2190,7 +2156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="22">
         <v>10</v>
       </c>
@@ -2206,183 +2172,183 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="22">
         <v>11</v>
       </c>
       <c r="B45" s="12"/>
       <c r="C45" s="12"/>
       <c r="D45" s="13"/>
-      <c r="E45" s="143"/>
-      <c r="F45" s="137"/>
-      <c r="G45" s="138"/>
+      <c r="E45" s="50"/>
+      <c r="F45" s="51"/>
+      <c r="G45" s="52"/>
       <c r="H45" s="14"/>
       <c r="I45" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="22">
         <v>12</v>
       </c>
       <c r="B46" s="12"/>
       <c r="C46" s="12"/>
       <c r="D46" s="13"/>
-      <c r="E46" s="143"/>
-      <c r="F46" s="137"/>
-      <c r="G46" s="138"/>
+      <c r="E46" s="50"/>
+      <c r="F46" s="51"/>
+      <c r="G46" s="52"/>
       <c r="H46" s="14"/>
       <c r="I46" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="22">
         <v>13</v>
       </c>
       <c r="B47" s="12"/>
       <c r="C47" s="12"/>
       <c r="D47" s="13"/>
-      <c r="E47" s="143"/>
-      <c r="F47" s="137"/>
-      <c r="G47" s="138"/>
+      <c r="E47" s="50"/>
+      <c r="F47" s="51"/>
+      <c r="G47" s="52"/>
       <c r="H47" s="14"/>
       <c r="I47" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="22">
         <v>14</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="12"/>
       <c r="D48" s="13"/>
-      <c r="E48" s="143"/>
-      <c r="F48" s="137"/>
-      <c r="G48" s="138"/>
+      <c r="E48" s="50"/>
+      <c r="F48" s="51"/>
+      <c r="G48" s="52"/>
       <c r="H48" s="14"/>
       <c r="I48" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="22">
         <v>15</v>
       </c>
       <c r="B49" s="12"/>
       <c r="C49" s="12"/>
       <c r="D49" s="13"/>
-      <c r="E49" s="143"/>
-      <c r="F49" s="137"/>
-      <c r="G49" s="138"/>
+      <c r="E49" s="50"/>
+      <c r="F49" s="51"/>
+      <c r="G49" s="52"/>
       <c r="H49" s="14"/>
       <c r="I49" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="22">
         <v>16</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="12"/>
       <c r="D50" s="13"/>
-      <c r="E50" s="143"/>
-      <c r="F50" s="137"/>
-      <c r="G50" s="138"/>
+      <c r="E50" s="50"/>
+      <c r="F50" s="51"/>
+      <c r="G50" s="52"/>
       <c r="H50" s="14"/>
       <c r="I50" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="22">
         <v>17</v>
       </c>
       <c r="B51" s="12"/>
       <c r="C51" s="12"/>
       <c r="D51" s="13"/>
-      <c r="E51" s="143"/>
-      <c r="F51" s="137"/>
-      <c r="G51" s="138"/>
+      <c r="E51" s="50"/>
+      <c r="F51" s="51"/>
+      <c r="G51" s="52"/>
       <c r="H51" s="14"/>
       <c r="I51" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="22">
         <v>18</v>
       </c>
       <c r="B52" s="12"/>
       <c r="C52" s="12"/>
       <c r="D52" s="13"/>
-      <c r="E52" s="143"/>
-      <c r="F52" s="137"/>
-      <c r="G52" s="138"/>
+      <c r="E52" s="50"/>
+      <c r="F52" s="51"/>
+      <c r="G52" s="52"/>
       <c r="H52" s="14"/>
       <c r="I52" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="22">
         <v>19</v>
       </c>
       <c r="B53" s="12"/>
       <c r="C53" s="12"/>
       <c r="D53" s="13"/>
-      <c r="E53" s="143"/>
-      <c r="F53" s="137"/>
-      <c r="G53" s="138"/>
+      <c r="E53" s="50"/>
+      <c r="F53" s="51"/>
+      <c r="G53" s="52"/>
       <c r="H53" s="14"/>
       <c r="I53" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="22">
         <v>20</v>
       </c>
       <c r="B54" s="15"/>
       <c r="C54" s="15"/>
       <c r="D54" s="15"/>
-      <c r="E54" s="144"/>
-      <c r="F54" s="145"/>
-      <c r="G54" s="146"/>
+      <c r="E54" s="71"/>
+      <c r="F54" s="72"/>
+      <c r="G54" s="73"/>
       <c r="H54" s="16"/>
       <c r="I54" s="23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="147" t="s">
+    <row r="55" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="B55" s="148"/>
-      <c r="C55" s="148"/>
-      <c r="D55" s="148"/>
-      <c r="E55" s="148"/>
-      <c r="F55" s="148"/>
-      <c r="G55" s="148"/>
-      <c r="H55" s="149"/>
+      <c r="B55" s="54"/>
+      <c r="C55" s="54"/>
+      <c r="D55" s="54"/>
+      <c r="E55" s="54"/>
+      <c r="F55" s="54"/>
+      <c r="G55" s="54"/>
+      <c r="H55" s="55"/>
       <c r="I55" s="24">
         <f>SUM(I35:I54)</f>
         <v>348.98</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="25"/>
       <c r="B56" s="26"/>
       <c r="C56" s="26"/>
@@ -2393,44 +2359,44 @@
       <c r="H56" s="26"/>
       <c r="I56" s="27"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="139" t="s">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A57" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="B57" s="140"/>
-      <c r="C57" s="140"/>
-      <c r="D57" s="140"/>
-      <c r="E57" s="141"/>
-      <c r="F57" s="141"/>
-      <c r="G57" s="141"/>
-      <c r="H57" s="141"/>
+      <c r="B57" s="68"/>
+      <c r="C57" s="68"/>
+      <c r="D57" s="68"/>
+      <c r="E57" s="69"/>
+      <c r="F57" s="69"/>
+      <c r="G57" s="69"/>
+      <c r="H57" s="69"/>
       <c r="I57" s="28"/>
     </row>
-    <row r="58" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="139"/>
-      <c r="B58" s="140"/>
-      <c r="C58" s="140"/>
-      <c r="D58" s="140"/>
-      <c r="E58" s="142"/>
-      <c r="F58" s="142"/>
-      <c r="G58" s="142"/>
-      <c r="H58" s="142"/>
+    <row r="58" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="67"/>
+      <c r="B58" s="68"/>
+      <c r="C58" s="68"/>
+      <c r="D58" s="68"/>
+      <c r="E58" s="70"/>
+      <c r="F58" s="70"/>
+      <c r="G58" s="70"/>
+      <c r="H58" s="70"/>
       <c r="I58" s="28"/>
     </row>
-    <row r="59" spans="1:9" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" ht="25.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="29"/>
       <c r="B59" s="30"/>
       <c r="C59" s="30"/>
       <c r="D59" s="30"/>
-      <c r="E59" s="130" t="s">
-        <v>44</v>
-      </c>
-      <c r="F59" s="130"/>
-      <c r="G59" s="130"/>
-      <c r="H59" s="130"/>
+      <c r="E59" s="60" t="s">
+        <v>43</v>
+      </c>
+      <c r="F59" s="60"/>
+      <c r="G59" s="60"/>
+      <c r="H59" s="60"/>
       <c r="I59" s="31"/>
     </row>
-    <row r="60" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A60" s="11"/>
       <c r="B60" s="11"/>
       <c r="C60" s="11"/>
@@ -2441,40 +2407,73 @@
       <c r="H60" s="11"/>
       <c r="I60" s="11"/>
     </row>
-    <row r="61" spans="1:9" s="11" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="126" t="s">
+    <row r="61" spans="1:9" s="11" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="B61" s="127"/>
-      <c r="C61" s="127"/>
-      <c r="D61" s="128"/>
+      <c r="B61" s="57"/>
+      <c r="C61" s="57"/>
+      <c r="D61" s="58"/>
       <c r="E61" s="32"/>
       <c r="F61" s="32"/>
       <c r="G61" s="32"/>
       <c r="H61" s="32"/>
       <c r="I61" s="33"/>
     </row>
-    <row r="62" spans="1:9" ht="150" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="131"/>
-      <c r="B62" s="132"/>
-      <c r="C62" s="132"/>
-      <c r="D62" s="132"/>
-      <c r="E62" s="132"/>
-      <c r="F62" s="132"/>
-      <c r="G62" s="132"/>
-      <c r="H62" s="132"/>
-      <c r="I62" s="133"/>
+    <row r="62" spans="1:9" ht="150" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="61"/>
+      <c r="B62" s="62"/>
+      <c r="C62" s="62"/>
+      <c r="D62" s="62"/>
+      <c r="E62" s="62"/>
+      <c r="F62" s="62"/>
+      <c r="G62" s="62"/>
+      <c r="H62" s="62"/>
+      <c r="I62" s="63"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0"/>
   <mergeCells count="63">
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="A55:H55"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="A14:I14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="A12:I12"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:H31"/>
+    <mergeCell ref="C23:H23"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C25:H25"/>
+    <mergeCell ref="C29:H29"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="A32:I32"/>
+    <mergeCell ref="A1:I3"/>
+    <mergeCell ref="A21:I21"/>
+    <mergeCell ref="A16:I16"/>
+    <mergeCell ref="A17:I17"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="A18:I18"/>
+    <mergeCell ref="A19:I19"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:I5"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="A6:I6"/>
+    <mergeCell ref="A7:I7"/>
+    <mergeCell ref="A8:I8"/>
     <mergeCell ref="A61:D61"/>
     <mergeCell ref="A33:I33"/>
     <mergeCell ref="E59:H59"/>
@@ -2491,46 +2490,13 @@
     <mergeCell ref="E54:G54"/>
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="E45:G45"/>
-    <mergeCell ref="A1:I3"/>
-    <mergeCell ref="A21:I21"/>
-    <mergeCell ref="A16:I16"/>
-    <mergeCell ref="A17:I17"/>
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="A18:I18"/>
-    <mergeCell ref="A19:I19"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:I5"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="A6:I6"/>
-    <mergeCell ref="A7:I7"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C31:H31"/>
-    <mergeCell ref="C23:H23"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="C25:H25"/>
-    <mergeCell ref="C29:H29"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="A32:I32"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C9:G9"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="A12:I12"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="A14:I14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:G15"/>
-    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="A55:H55"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="E51:G51"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <dataValidations count="1">

</xml_diff>